<commit_message>
Updated removed chromedriver.exe file not required now
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/PortFolioTest.xlsx
+++ b/src/main/resources/excel/PortFolioTest.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UltimateFramework\src\main\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UltiMateProject\UltimateFramework\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADDE9220-2048-42A9-ADB3-827E566058DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D59C86F-84AE-461D-94CF-7F90D2AF7BE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="19406" windowHeight="11606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="19406" windowHeight="11606" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCase" sheetId="1" r:id="rId1"/>
@@ -321,7 +321,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -540,13 +540,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="20.84375" customWidth="1"/>
+    <col min="1" max="1" width="27" customWidth="1"/>
     <col min="2" max="2" width="15.4609375" customWidth="1"/>
     <col min="3" max="6" width="8.69140625" customWidth="1"/>
   </cols>
@@ -572,7 +572,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.6" x14ac:dyDescent="0.4">
@@ -580,7 +580,7 @@
         <v>46</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="14.6" x14ac:dyDescent="0.4">
@@ -588,7 +588,7 @@
         <v>52</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="14.6" x14ac:dyDescent="0.4">
@@ -596,7 +596,7 @@
         <v>53</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.4">
@@ -604,7 +604,7 @@
         <v>54</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1597,8 +1597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M1000"/>
   <sheetViews>
-    <sheetView zoomScale="79" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="79" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1781,7 +1781,7 @@
     </row>
     <row r="11" spans="1:13" ht="14.6" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>45</v>
@@ -1967,7 +1967,7 @@
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
@@ -1985,7 +1985,7 @@
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
@@ -2003,7 +2003,7 @@
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">

</xml_diff>